<commit_message>
feat(small_df_model.py): update dataset and input files
The dataset file used in 'small_df_model.py' has been updated from
'Training_reference.xlsx' to 'Training_a.xlsx'. Similarly, the input
file has been changed from 'input_descriptions_and_suppliers.xlsm' to
'inputs_b.xlsx'. Also, a minor change has been made in the
'get_combined_description_supplier' function where the unused variable
'_index' has been replaced with '_'.
</commit_message>
<xml_diff>
--- a/results/predicted_unspsc_results.xlsx
+++ b/results/predicted_unspsc_results.xlsx
@@ -468,22 +468,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>N43222600</t>
+          <t>N23261601</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Network service equipment</t>
+          <t>Three dimensional printing filament</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>BSP-ITT-CATL4-218</t>
+          <t>MSP-AM-CATL4-962</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>NETWORK MISCELLANOUS HARDWARE</t>
+          <t>ADDITIVE PRINTING MATERIALS / OTHER</t>
         </is>
       </c>
     </row>
@@ -522,22 +522,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>N43222600</t>
+          <t>N23261601</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Network service equipment</t>
+          <t>Three dimensional printing filament</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>BSP-ITT-CATL4-218</t>
+          <t>MSP-AM-CATL4-962</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>NETWORK MISCELLANOUS HARDWARE</t>
+          <t>ADDITIVE PRINTING MATERIALS / OTHER</t>
         </is>
       </c>
     </row>
@@ -549,22 +549,22 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>N43222600</t>
+          <t>N23261601</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Network service equipment</t>
+          <t>Three dimensional printing filament</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>BSP-ITT-CATL4-218</t>
+          <t>MSP-AM-CATL4-962</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>NETWORK MISCELLANOUS HARDWARE</t>
+          <t>ADDITIVE PRINTING MATERIALS / OTHER</t>
         </is>
       </c>
     </row>
@@ -576,22 +576,22 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>N44122002</t>
+          <t>N23261601</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Sheet protectors</t>
+          <t>Three dimensional printing filament</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>BSP-HRES-CATL4-039</t>
+          <t>MSP-AM-CATL4-962</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>GENERAL OFFICE SUPPLIES</t>
+          <t>ADDITIVE PRINTING MATERIALS / OTHER</t>
         </is>
       </c>
     </row>
@@ -603,22 +603,22 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>N43222600</t>
+          <t>N23261601</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Network service equipment</t>
+          <t>Three dimensional printing filament</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>BSP-ITT-CATL4-218</t>
+          <t>MSP-AM-CATL4-962</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>NETWORK MISCELLANOUS HARDWARE</t>
+          <t>ADDITIVE PRINTING MATERIALS / OTHER</t>
         </is>
       </c>
     </row>
@@ -630,22 +630,22 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>N43222600</t>
+          <t>N23261601</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Network service equipment</t>
+          <t>Three dimensional printing filament</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>BSP-ITT-CATL4-218</t>
+          <t>MSP-AM-CATL4-962</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>NETWORK MISCELLANOUS HARDWARE</t>
+          <t>ADDITIVE PRINTING MATERIALS / OTHER</t>
         </is>
       </c>
     </row>
@@ -657,22 +657,22 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>N43222600</t>
+          <t>N23261601</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Network service equipment</t>
+          <t>Three dimensional printing filament</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>BSP-ITT-CATL4-218</t>
+          <t>MSP-AM-CATL4-962</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>NETWORK MISCELLANOUS HARDWARE</t>
+          <t>ADDITIVE PRINTING MATERIALS / OTHER</t>
         </is>
       </c>
     </row>
@@ -684,22 +684,22 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>N43222600</t>
+          <t>N23261601</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Network service equipment</t>
+          <t>Three dimensional printing filament</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>BSP-ITT-CATL4-218</t>
+          <t>MSP-AM-CATL4-962</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>NETWORK MISCELLANOUS HARDWARE</t>
+          <t>ADDITIVE PRINTING MATERIALS / OTHER</t>
         </is>
       </c>
     </row>
@@ -711,22 +711,22 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>N43222600</t>
+          <t>N23261601</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Network service equipment</t>
+          <t>Three dimensional printing filament</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>BSP-ITT-CATL4-218</t>
+          <t>MSP-AM-CATL4-962</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>NETWORK MISCELLANOUS HARDWARE</t>
+          <t>ADDITIVE PRINTING MATERIALS / OTHER</t>
         </is>
       </c>
     </row>
@@ -738,22 +738,22 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>N43222600</t>
+          <t>N23261601</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Network service equipment</t>
+          <t>Three dimensional printing filament</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>BSP-ITT-CATL4-218</t>
+          <t>MSP-AM-CATL4-962</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>NETWORK MISCELLANOUS HARDWARE</t>
+          <t>ADDITIVE PRINTING MATERIALS / OTHER</t>
         </is>
       </c>
     </row>
@@ -765,22 +765,22 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>N23260000</t>
+          <t>N23261600</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Rapid prototyping machinery and accessories</t>
+          <t>Rapid prototyping machine accessories</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>MSP-PES-CATL4-872</t>
+          <t>MSP-AM-CATL4-956</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>R&amp;D FIELD TEST MATERIALS CONSUMED</t>
+          <t>ADDITIVE PRINTING MATERIALS  - PLASTIC SPOOL</t>
         </is>
       </c>
     </row>
@@ -792,22 +792,22 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>N44103105</t>
+          <t>N23261600</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Ink cartridges</t>
+          <t>Rapid prototyping machine accessories</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Category Code not found</t>
+          <t>MSP-AM-CATL4-956</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Category Description not found</t>
+          <t>ADDITIVE PRINTING MATERIALS  - PLASTIC SPOOL</t>
         </is>
       </c>
     </row>
@@ -819,22 +819,22 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>N44122101</t>
+          <t>N23261601</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Rubber bands</t>
+          <t>Three dimensional printing filament</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>BSP-HRES-CATL4-039</t>
+          <t>MSP-AM-CATL4-962</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>GENERAL OFFICE SUPPLIES</t>
+          <t>ADDITIVE PRINTING MATERIALS / OTHER</t>
         </is>
       </c>
     </row>
@@ -846,22 +846,22 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>N55121611</t>
+          <t>N23261601</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Label making tapes</t>
+          <t>Three dimensional printing filament</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>MSP-PFE-CATL4-800</t>
+          <t>MSP-AM-CATL4-962</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>SEALANTS &amp; ADHESIVES</t>
+          <t>ADDITIVE PRINTING MATERIALS / OTHER</t>
         </is>
       </c>
     </row>
@@ -873,22 +873,22 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>N47131805</t>
+          <t>N23261601</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>General purpose cleaners</t>
+          <t>Three dimensional printing filament</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>MSP-FM-CATL4-645</t>
+          <t>MSP-AM-CATL4-962</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>CLEANING SUPPLIES</t>
+          <t>ADDITIVE PRINTING MATERIALS / OTHER</t>
         </is>
       </c>
     </row>
@@ -900,22 +900,22 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>N14111537</t>
+          <t>N23261601</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Label papers</t>
+          <t>Three dimensional printing filament</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>BSP-HRES-CATL4-039</t>
+          <t>MSP-AM-CATL4-962</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>GENERAL OFFICE SUPPLIES</t>
+          <t>ADDITIVE PRINTING MATERIALS / OTHER</t>
         </is>
       </c>
     </row>
@@ -927,22 +927,22 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>N44121716</t>
+          <t>N23261601</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Highlighters</t>
+          <t>Three dimensional printing filament</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>BSP-HRES-CATL4-039</t>
+          <t>MSP-AM-CATL4-962</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>GENERAL OFFICE SUPPLIES</t>
+          <t>ADDITIVE PRINTING MATERIALS / OTHER</t>
         </is>
       </c>
     </row>
@@ -954,22 +954,22 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>N44103500</t>
+          <t>N23261601</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Binding machine supplies</t>
+          <t>Three dimensional printing filament</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Category Code not found</t>
+          <t>MSP-AM-CATL4-962</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Category Description not found</t>
+          <t>ADDITIVE PRINTING MATERIALS / OTHER</t>
         </is>
       </c>
     </row>
@@ -981,22 +981,22 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>N55121611</t>
+          <t>N23261600</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Label making tapes</t>
+          <t>Rapid prototyping machine accessories</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>MSP-PFE-CATL4-800</t>
+          <t>MSP-AM-CATL4-956</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>SEALANTS &amp; ADHESIVES</t>
+          <t>ADDITIVE PRINTING MATERIALS  - PLASTIC SPOOL</t>
         </is>
       </c>
     </row>
@@ -1008,22 +1008,22 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>N56101720</t>
+          <t>N23261600</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Office or work chair</t>
+          <t>Rapid prototyping machine accessories</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>MSP-FM-CATL4-598</t>
+          <t>MSP-AM-CATL4-956</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>OFFICE FURNITURE</t>
+          <t>ADDITIVE PRINTING MATERIALS  - PLASTIC SPOOL</t>
         </is>
       </c>
     </row>
@@ -1035,22 +1035,22 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>N45100000</t>
+          <t>N23261601</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Printing and publishing equipment</t>
+          <t>Three dimensional printing filament</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Category Code not found</t>
+          <t>MSP-AM-CATL4-962</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Category Description not found</t>
+          <t>ADDITIVE PRINTING MATERIALS / OTHER</t>
         </is>
       </c>
     </row>
@@ -1062,22 +1062,22 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>N45100000</t>
+          <t>N23261601</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Printing and publishing equipment</t>
+          <t>Three dimensional printing filament</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Category Code not found</t>
+          <t>MSP-AM-CATL4-962</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Category Description not found</t>
+          <t>ADDITIVE PRINTING MATERIALS / OTHER</t>
         </is>
       </c>
     </row>
@@ -1089,22 +1089,22 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>N46182200</t>
+          <t>N23261600</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Ergonomic support aids</t>
+          <t>Rapid prototyping machine accessories</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>MSP-FM-CATL4-926</t>
+          <t>MSP-AM-CATL4-956</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>OTHER SAFETY SUPPLIES</t>
+          <t>ADDITIVE PRINTING MATERIALS  - PLASTIC SPOOL</t>
         </is>
       </c>
     </row>
@@ -1116,22 +1116,22 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>N46181700</t>
+          <t>N23261600</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Face and head protection</t>
+          <t>Rapid prototyping machine accessories</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>MSP-FM-CATL4-924</t>
+          <t>MSP-AM-CATL4-956</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>SAFETY CLOTHES</t>
+          <t>ADDITIVE PRINTING MATERIALS  - PLASTIC SPOOL</t>
         </is>
       </c>
     </row>
@@ -1143,12 +1143,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>N39121031</t>
+          <t>N39121004</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Power supply outlet strip</t>
+          <t>Power supply units</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1170,22 +1170,22 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>N24100000</t>
+          <t>N23261600</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Material handling machinery and equipment</t>
+          <t>Rapid prototyping machine accessories</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>MSP-FWA-CATL4-502</t>
+          <t>MSP-AM-CATL4-956</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>MANUAL GUIDED VEHICLE (MGV)</t>
+          <t>ADDITIVE PRINTING MATERIALS  - PLASTIC SPOOL</t>
         </is>
       </c>
     </row>
@@ -1197,22 +1197,22 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>N23260000</t>
+          <t>N23261600</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Rapid prototyping machinery and accessories</t>
+          <t>Rapid prototyping machine accessories</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>MSP-PES-CATL4-872</t>
+          <t>MSP-AM-CATL4-956</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>R&amp;D FIELD TEST MATERIALS CONSUMED</t>
+          <t>ADDITIVE PRINTING MATERIALS  - PLASTIC SPOOL</t>
         </is>
       </c>
     </row>
@@ -1224,22 +1224,22 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>N43211609</t>
+          <t>N43211600</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Universal serial bus hubs or connectors</t>
+          <t>Computer accessories</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Category Code not found</t>
+          <t>BSP-ITT-CATL4-123</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Category Description not found</t>
+          <t>SHOP FLOOR ACCESSORIES</t>
         </is>
       </c>
     </row>
@@ -1251,22 +1251,22 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>N43211724</t>
+          <t>N27112700</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Computer peripheral kit</t>
+          <t>Power tools</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Category Code not found</t>
+          <t>MSP-FWA-CATL4-557</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Category Description not found</t>
+          <t>TORQUE TOOLS - DATA COLLECTING</t>
         </is>
       </c>
     </row>
@@ -1278,22 +1278,22 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>N43202222</t>
+          <t>N26121500</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Computer cable</t>
+          <t>Electrical wire</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Category Code not found</t>
+          <t>MSP-FM-CATL4-629</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Category Description not found</t>
+          <t>FACILITIES REPAIR - ELECTRICAL MATERIALS</t>
         </is>
       </c>
     </row>
@@ -1332,22 +1332,22 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>N43211800</t>
+          <t>N43191600</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Computer data input device accessories</t>
+          <t>Personal communications device accessories or parts</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Category Code not found</t>
+          <t>MSP-FM-CATL4-596</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Category Description not found</t>
+          <t>COMMUNICATION EQUIPMENT</t>
         </is>
       </c>
     </row>
@@ -1359,22 +1359,22 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>N47131805</t>
+          <t>N44111506</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>General purpose cleaners</t>
+          <t>Paper or pad holder or dispensers</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>MSP-FM-CATL4-645</t>
+          <t>BSP-HRES-CATL4-039</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>CLEANING SUPPLIES</t>
+          <t>GENERAL OFFICE SUPPLIES</t>
         </is>
       </c>
     </row>
@@ -1386,22 +1386,22 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>N43201404</t>
+          <t>N15121529</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Network interface cards</t>
+          <t>Refrigerating machine oil</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Category Code not found</t>
+          <t>MSP-PFE-CATL4-814</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Category Description not found</t>
+          <t>COOLANT MACHINING</t>
         </is>
       </c>
     </row>
@@ -1413,22 +1413,22 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>N43211802</t>
+          <t>N39101600</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Mouse pads</t>
+          <t>Lamps and lightbulbs</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Category Code not found</t>
+          <t>MSP-FM-CATL4-629</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Category Description not found</t>
+          <t>FACILITIES REPAIR - ELECTRICAL MATERIALS</t>
         </is>
       </c>
     </row>
@@ -1440,22 +1440,22 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>N43211724</t>
+          <t>N45121500</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Computer peripheral kit</t>
+          <t>Cameras</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Category Code not found</t>
+          <t>BSP-HRES-CATL4-039</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Category Description not found</t>
+          <t>GENERAL OFFICE SUPPLIES</t>
         </is>
       </c>
     </row>
@@ -1467,22 +1467,22 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>N31201517</t>
+          <t>N24121500</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Packaging tape</t>
+          <t>Packaging boxes and bags and pouches</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>MSP-WWP-CATL4-986</t>
+          <t>MSP-WWP-CATL4-976</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>TAPES</t>
+          <t>CHIPBOARD</t>
         </is>
       </c>
     </row>
@@ -1494,22 +1494,22 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>N47131805</t>
+          <t>N44111506</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>General purpose cleaners</t>
+          <t>Paper or pad holder or dispensers</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>MSP-FM-CATL4-645</t>
+          <t>BSP-HRES-CATL4-039</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>CLEANING SUPPLIES</t>
+          <t>GENERAL OFFICE SUPPLIES</t>
         </is>
       </c>
     </row>
@@ -1521,22 +1521,22 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>N47131805</t>
+          <t>N44111506</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>General purpose cleaners</t>
+          <t>Paper or pad holder or dispensers</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>MSP-FM-CATL4-645</t>
+          <t>BSP-HRES-CATL4-039</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>CLEANING SUPPLIES</t>
+          <t>GENERAL OFFICE SUPPLIES</t>
         </is>
       </c>
     </row>
@@ -1548,22 +1548,22 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>N47131805</t>
+          <t>N24122001</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>General purpose cleaners</t>
+          <t>Squeeze bottles</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>MSP-FM-CATL4-645</t>
+          <t>MSP-WWP-CATL4-982</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>CLEANING SUPPLIES</t>
+          <t>PACKAGING ACCESSORIES MISCELLANEOUS</t>
         </is>
       </c>
     </row>
@@ -1575,22 +1575,22 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>N43202222</t>
+          <t>N39131700</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Computer cable</t>
+          <t>Wire Raceways Conduit and Busways</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Category Code not found</t>
+          <t>MSP-FM-CATL4-629</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Category Description not found</t>
+          <t>FACILITIES REPAIR - ELECTRICAL MATERIALS</t>
         </is>
       </c>
     </row>
@@ -1602,22 +1602,22 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>N43202222</t>
+          <t>N39131700</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Computer cable</t>
+          <t>Wire Raceways Conduit and Busways</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Category Code not found</t>
+          <t>MSP-FM-CATL4-629</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Category Description not found</t>
+          <t>FACILITIES REPAIR - ELECTRICAL MATERIALS</t>
         </is>
       </c>
     </row>
@@ -1629,22 +1629,22 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>N47131805</t>
+          <t>N24122001</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>General purpose cleaners</t>
+          <t>Squeeze bottles</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>MSP-FM-CATL4-645</t>
+          <t>MSP-WWP-CATL4-982</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>CLEANING SUPPLIES</t>
+          <t>PACKAGING ACCESSORIES MISCELLANEOUS</t>
         </is>
       </c>
     </row>
@@ -1656,22 +1656,22 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>N31201517</t>
+          <t>N24121500</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Packaging tape</t>
+          <t>Packaging boxes and bags and pouches</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>MSP-WWP-CATL4-986</t>
+          <t>MSP-WWP-CATL4-976</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>TAPES</t>
+          <t>CHIPBOARD</t>
         </is>
       </c>
     </row>
@@ -1683,22 +1683,22 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>N31201517</t>
+          <t>N24121500</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Packaging tape</t>
+          <t>Packaging boxes and bags and pouches</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>MSP-WWP-CATL4-986</t>
+          <t>MSP-WWP-CATL4-976</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>TAPES</t>
+          <t>CHIPBOARD</t>
         </is>
       </c>
     </row>
@@ -1710,22 +1710,22 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>N31201517</t>
+          <t>N24121500</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Packaging tape</t>
+          <t>Packaging boxes and bags and pouches</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>MSP-WWP-CATL4-986</t>
+          <t>MSP-WWP-CATL4-976</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>TAPES</t>
+          <t>CHIPBOARD</t>
         </is>
       </c>
     </row>
@@ -1791,22 +1791,22 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>N43222612</t>
+          <t>N78100000</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Network switches</t>
+          <t>Mail and cargo transport</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>BSP-ITT-CATL4-219</t>
+          <t>LSP-WWLAPEX-CATL2-021</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>NETWORK SWITCHES / ROUTERS</t>
+          <t>AIR, PARCEL, EXPRESS, GLOBAL TRADE SERVICES</t>
         </is>
       </c>
     </row>
@@ -1818,22 +1818,22 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>N43222612</t>
+          <t>N78100000</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Network switches</t>
+          <t>Mail and cargo transport</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>BSP-ITT-CATL4-219</t>
+          <t>LSP-WWLAPEX-CATL2-021</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>NETWORK SWITCHES / ROUTERS</t>
+          <t>AIR, PARCEL, EXPRESS, GLOBAL TRADE SERVICES</t>
         </is>
       </c>
     </row>
@@ -1845,22 +1845,22 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>N43222612</t>
+          <t>N78100000</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Network switches</t>
+          <t>Mail and cargo transport</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>BSP-ITT-CATL4-219</t>
+          <t>LSP-WWLAPEX-CATL2-021</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>NETWORK SWITCHES / ROUTERS</t>
+          <t>AIR, PARCEL, EXPRESS, GLOBAL TRADE SERVICES</t>
         </is>
       </c>
     </row>
@@ -1872,22 +1872,22 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>N43222612</t>
+          <t>N78100000</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Network switches</t>
+          <t>Mail and cargo transport</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>BSP-ITT-CATL4-219</t>
+          <t>LSP-WWLAPEX-CATL2-021</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>NETWORK SWITCHES / ROUTERS</t>
+          <t>AIR, PARCEL, EXPRESS, GLOBAL TRADE SERVICES</t>
         </is>
       </c>
     </row>
@@ -1899,22 +1899,22 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>N43222612</t>
+          <t>N78100000</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Network switches</t>
+          <t>Mail and cargo transport</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>BSP-ITT-CATL4-219</t>
+          <t>LSP-WWLAPEX-CATL2-021</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>NETWORK SWITCHES / ROUTERS</t>
+          <t>AIR, PARCEL, EXPRESS, GLOBAL TRADE SERVICES</t>
         </is>
       </c>
     </row>
@@ -1926,22 +1926,22 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>N43222612</t>
+          <t>N78100000</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Network switches</t>
+          <t>Mail and cargo transport</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>BSP-ITT-CATL4-219</t>
+          <t>LSP-WWLAPEX-CATL2-021</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>NETWORK SWITCHES / ROUTERS</t>
+          <t>AIR, PARCEL, EXPRESS, GLOBAL TRADE SERVICES</t>
         </is>
       </c>
     </row>
@@ -1953,22 +1953,22 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>N43222612</t>
+          <t>N78100000</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Network switches</t>
+          <t>Mail and cargo transport</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>BSP-ITT-CATL4-219</t>
+          <t>LSP-WWLAPEX-CATL2-021</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>NETWORK SWITCHES / ROUTERS</t>
+          <t>AIR, PARCEL, EXPRESS, GLOBAL TRADE SERVICES</t>
         </is>
       </c>
     </row>
@@ -1980,22 +1980,22 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>N43222612</t>
+          <t>N78100000</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Network switches</t>
+          <t>Mail and cargo transport</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>BSP-ITT-CATL4-219</t>
+          <t>LSP-WWLAPEX-CATL2-021</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>NETWORK SWITCHES / ROUTERS</t>
+          <t>AIR, PARCEL, EXPRESS, GLOBAL TRADE SERVICES</t>
         </is>
       </c>
     </row>
@@ -2007,22 +2007,22 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>N43222612</t>
+          <t>N78100000</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Network switches</t>
+          <t>Mail and cargo transport</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>BSP-ITT-CATL4-219</t>
+          <t>LSP-WWLAPEX-CATL2-021</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>NETWORK SWITCHES / ROUTERS</t>
+          <t>AIR, PARCEL, EXPRESS, GLOBAL TRADE SERVICES</t>
         </is>
       </c>
     </row>
@@ -2034,22 +2034,22 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>N43222612</t>
+          <t>N78100000</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Network switches</t>
+          <t>Mail and cargo transport</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>BSP-ITT-CATL4-219</t>
+          <t>LSP-WWLAPEX-CATL2-021</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>NETWORK SWITCHES / ROUTERS</t>
+          <t>AIR, PARCEL, EXPRESS, GLOBAL TRADE SERVICES</t>
         </is>
       </c>
     </row>
@@ -2061,22 +2061,22 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>N78141501</t>
+          <t>N78121603</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Freight forwarders services</t>
+          <t>Freight fee</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>LSP-APEX-CATL4-296</t>
+          <t>LSP-WWLOWS-CATL4-323</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>FREIGHT FORWARDING</t>
+          <t>HANDLING FEES, WHSE</t>
         </is>
       </c>
     </row>
@@ -2088,22 +2088,22 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>N44121500</t>
+          <t>N24121500</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Mailing supplies</t>
+          <t>Packaging boxes and bags and pouches</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>BSP-HRES-CATL4-040</t>
+          <t>MSP-WWP-CATL4-976</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>MAILROOM EQUIPMENT AND SUPPLIES</t>
+          <t>CHIPBOARD</t>
         </is>
       </c>
     </row>
@@ -2115,22 +2115,22 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>N24111514</t>
+          <t>N50161800</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Zipper bag</t>
+          <t>Confectionary products</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Category Code not found</t>
+          <t>BSP-HRES-CATL4-030</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Category Description not found</t>
+          <t>CAFETERIA SERVICES</t>
         </is>
       </c>
     </row>
@@ -2142,22 +2142,22 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>N24121500</t>
+          <t>N24121502</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Packaging boxes and bags and pouches</t>
+          <t>Packaging pouches or bags</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>MSP-WWP-CATL4-976</t>
+          <t>MSP-WWP-CATL4-983</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>CHIPBOARD</t>
+          <t>PLASTIC BAGS</t>
         </is>
       </c>
     </row>
@@ -2169,22 +2169,22 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>N50202300</t>
+          <t>N78141500</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Non alcoholic beverages</t>
+          <t>Transport arranging services</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>BSP-HRES-CATL4-030</t>
+          <t>LSP-WWLAPEX-CATL2-021</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>CAFETERIA SERVICES</t>
+          <t>AIR, PARCEL, EXPRESS, GLOBAL TRADE SERVICES</t>
         </is>
       </c>
     </row>
@@ -2223,22 +2223,22 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>N47131805</t>
+          <t>N44111506</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>General purpose cleaners</t>
+          <t>Paper or pad holder or dispensers</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>MSP-FM-CATL4-645</t>
+          <t>BSP-HRES-CATL4-039</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>CLEANING SUPPLIES</t>
+          <t>GENERAL OFFICE SUPPLIES</t>
         </is>
       </c>
     </row>
@@ -2250,22 +2250,22 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>N24111514</t>
+          <t>N41110000</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Zipper bag</t>
+          <t>Measuring and observing and testing instruments</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Category Code not found</t>
+          <t>MSP-FWA-CATL4-415</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Category Description not found</t>
+          <t>FLOW METERS</t>
         </is>
       </c>
     </row>
@@ -2277,22 +2277,22 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>N14111601</t>
+          <t>N24121502</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Gift wrapping paper or bags or boxes</t>
+          <t>Packaging pouches or bags</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>BSP-HRES-CATL4-039</t>
+          <t>MSP-WWP-CATL4-983</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>GENERAL OFFICE SUPPLIES</t>
+          <t>PLASTIC BAGS</t>
         </is>
       </c>
     </row>
@@ -2304,22 +2304,22 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>N47131805</t>
+          <t>N24122001</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>General purpose cleaners</t>
+          <t>Squeeze bottles</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>MSP-FM-CATL4-645</t>
+          <t>MSP-WWP-CATL4-982</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>CLEANING SUPPLIES</t>
+          <t>PACKAGING ACCESSORIES MISCELLANEOUS</t>
         </is>
       </c>
     </row>
@@ -2331,22 +2331,22 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>N47131805</t>
+          <t>N44111506</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>General purpose cleaners</t>
+          <t>Paper or pad holder or dispensers</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>MSP-FM-CATL4-645</t>
+          <t>BSP-HRES-CATL4-039</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>CLEANING SUPPLIES</t>
+          <t>GENERAL OFFICE SUPPLIES</t>
         </is>
       </c>
     </row>
@@ -2358,22 +2358,22 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>N47131805</t>
+          <t>N44111506</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>General purpose cleaners</t>
+          <t>Paper or pad holder or dispensers</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>MSP-FM-CATL4-645</t>
+          <t>BSP-HRES-CATL4-039</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>CLEANING SUPPLIES</t>
+          <t>GENERAL OFFICE SUPPLIES</t>
         </is>
       </c>
     </row>
@@ -2385,22 +2385,22 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>N47131805</t>
+          <t>N44111506</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>General purpose cleaners</t>
+          <t>Paper or pad holder or dispensers</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>MSP-FM-CATL4-645</t>
+          <t>BSP-HRES-CATL4-039</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>CLEANING SUPPLIES</t>
+          <t>GENERAL OFFICE SUPPLIES</t>
         </is>
       </c>
     </row>
@@ -2412,22 +2412,22 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>N47131805</t>
+          <t>N44111506</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>General purpose cleaners</t>
+          <t>Paper or pad holder or dispensers</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>MSP-FM-CATL4-645</t>
+          <t>BSP-HRES-CATL4-039</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>CLEANING SUPPLIES</t>
+          <t>GENERAL OFFICE SUPPLIES</t>
         </is>
       </c>
     </row>
@@ -2439,22 +2439,22 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>N47131805</t>
+          <t>N44111506</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>General purpose cleaners</t>
+          <t>Paper or pad holder or dispensers</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>MSP-FM-CATL4-645</t>
+          <t>BSP-HRES-CATL4-039</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>CLEANING SUPPLIES</t>
+          <t>GENERAL OFFICE SUPPLIES</t>
         </is>
       </c>
     </row>
@@ -2466,22 +2466,22 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>N47131805</t>
+          <t>N44111506</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>General purpose cleaners</t>
+          <t>Paper or pad holder or dispensers</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>MSP-FM-CATL4-645</t>
+          <t>BSP-HRES-CATL4-039</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>CLEANING SUPPLIES</t>
+          <t>GENERAL OFFICE SUPPLIES</t>
         </is>
       </c>
     </row>
@@ -2493,22 +2493,22 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>N47131805</t>
+          <t>N44111506</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>General purpose cleaners</t>
+          <t>Paper or pad holder or dispensers</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>MSP-FM-CATL4-645</t>
+          <t>BSP-HRES-CATL4-039</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>CLEANING SUPPLIES</t>
+          <t>GENERAL OFFICE SUPPLIES</t>
         </is>
       </c>
     </row>
@@ -2520,22 +2520,22 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>N47131805</t>
+          <t>N44111506</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>General purpose cleaners</t>
+          <t>Paper or pad holder or dispensers</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>MSP-FM-CATL4-645</t>
+          <t>BSP-HRES-CATL4-039</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>CLEANING SUPPLIES</t>
+          <t>GENERAL OFFICE SUPPLIES</t>
         </is>
       </c>
     </row>
@@ -2547,22 +2547,22 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>N47131805</t>
+          <t>N44111506</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>General purpose cleaners</t>
+          <t>Paper or pad holder or dispensers</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>MSP-FM-CATL4-645</t>
+          <t>BSP-HRES-CATL4-039</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>CLEANING SUPPLIES</t>
+          <t>GENERAL OFFICE SUPPLIES</t>
         </is>
       </c>
     </row>
@@ -2574,22 +2574,22 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>N47131805</t>
+          <t>N44111506</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>General purpose cleaners</t>
+          <t>Paper or pad holder or dispensers</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>MSP-FM-CATL4-645</t>
+          <t>BSP-HRES-CATL4-039</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>CLEANING SUPPLIES</t>
+          <t>GENERAL OFFICE SUPPLIES</t>
         </is>
       </c>
     </row>
@@ -2601,22 +2601,22 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>N47131805</t>
+          <t>N44111506</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>General purpose cleaners</t>
+          <t>Paper or pad holder or dispensers</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>MSP-FM-CATL4-645</t>
+          <t>BSP-HRES-CATL4-039</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>CLEANING SUPPLIES</t>
+          <t>GENERAL OFFICE SUPPLIES</t>
         </is>
       </c>
     </row>
@@ -2628,22 +2628,22 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>N47131805</t>
+          <t>N44111506</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>General purpose cleaners</t>
+          <t>Paper or pad holder or dispensers</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>MSP-FM-CATL4-645</t>
+          <t>BSP-HRES-CATL4-039</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>CLEANING SUPPLIES</t>
+          <t>GENERAL OFFICE SUPPLIES</t>
         </is>
       </c>
     </row>
@@ -2655,22 +2655,22 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>N47131805</t>
+          <t>N44111506</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>General purpose cleaners</t>
+          <t>Paper or pad holder or dispensers</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>MSP-FM-CATL4-645</t>
+          <t>BSP-HRES-CATL4-039</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>CLEANING SUPPLIES</t>
+          <t>GENERAL OFFICE SUPPLIES</t>
         </is>
       </c>
     </row>
@@ -2682,22 +2682,22 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>N47131805</t>
+          <t>N44111506</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>General purpose cleaners</t>
+          <t>Paper or pad holder or dispensers</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>MSP-FM-CATL4-645</t>
+          <t>BSP-HRES-CATL4-039</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>CLEANING SUPPLIES</t>
+          <t>GENERAL OFFICE SUPPLIES</t>
         </is>
       </c>
     </row>
@@ -2709,22 +2709,22 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>N47131805</t>
+          <t>N44111506</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>General purpose cleaners</t>
+          <t>Paper or pad holder or dispensers</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>MSP-FM-CATL4-645</t>
+          <t>BSP-HRES-CATL4-039</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>CLEANING SUPPLIES</t>
+          <t>GENERAL OFFICE SUPPLIES</t>
         </is>
       </c>
     </row>
@@ -2736,22 +2736,22 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>N47131805</t>
+          <t>N44111506</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>General purpose cleaners</t>
+          <t>Paper or pad holder or dispensers</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>MSP-FM-CATL4-645</t>
+          <t>BSP-HRES-CATL4-039</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>CLEANING SUPPLIES</t>
+          <t>GENERAL OFFICE SUPPLIES</t>
         </is>
       </c>
     </row>
@@ -2763,22 +2763,22 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>N47131805</t>
+          <t>N44111506</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>General purpose cleaners</t>
+          <t>Paper or pad holder or dispensers</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>MSP-FM-CATL4-645</t>
+          <t>BSP-HRES-CATL4-039</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>CLEANING SUPPLIES</t>
+          <t>GENERAL OFFICE SUPPLIES</t>
         </is>
       </c>
     </row>
@@ -2790,22 +2790,22 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>N47131805</t>
+          <t>N44111506</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>General purpose cleaners</t>
+          <t>Paper or pad holder or dispensers</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>MSP-FM-CATL4-645</t>
+          <t>BSP-HRES-CATL4-039</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>CLEANING SUPPLIES</t>
+          <t>GENERAL OFFICE SUPPLIES</t>
         </is>
       </c>
     </row>
@@ -2817,22 +2817,22 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>N47131805</t>
+          <t>N44111506</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>General purpose cleaners</t>
+          <t>Paper or pad holder or dispensers</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>MSP-FM-CATL4-645</t>
+          <t>BSP-HRES-CATL4-039</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>CLEANING SUPPLIES</t>
+          <t>GENERAL OFFICE SUPPLIES</t>
         </is>
       </c>
     </row>
@@ -2844,22 +2844,22 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>N47131805</t>
+          <t>N44111506</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>General purpose cleaners</t>
+          <t>Paper or pad holder or dispensers</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>MSP-FM-CATL4-645</t>
+          <t>BSP-HRES-CATL4-039</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>CLEANING SUPPLIES</t>
+          <t>GENERAL OFFICE SUPPLIES</t>
         </is>
       </c>
     </row>
@@ -2871,22 +2871,22 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>N47131805</t>
+          <t>N44111506</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>General purpose cleaners</t>
+          <t>Paper or pad holder or dispensers</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>MSP-FM-CATL4-645</t>
+          <t>BSP-HRES-CATL4-039</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>CLEANING SUPPLIES</t>
+          <t>GENERAL OFFICE SUPPLIES</t>
         </is>
       </c>
     </row>
@@ -2898,22 +2898,22 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>N47131805</t>
+          <t>N44111506</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>General purpose cleaners</t>
+          <t>Paper or pad holder or dispensers</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>MSP-FM-CATL4-645</t>
+          <t>BSP-HRES-CATL4-039</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>CLEANING SUPPLIES</t>
+          <t>GENERAL OFFICE SUPPLIES</t>
         </is>
       </c>
     </row>
@@ -2925,22 +2925,22 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>N47131805</t>
+          <t>N44111506</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>General purpose cleaners</t>
+          <t>Paper or pad holder or dispensers</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>MSP-FM-CATL4-645</t>
+          <t>BSP-HRES-CATL4-039</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>CLEANING SUPPLIES</t>
+          <t>GENERAL OFFICE SUPPLIES</t>
         </is>
       </c>
     </row>
@@ -2952,22 +2952,22 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>N47131805</t>
+          <t>N44111506</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>General purpose cleaners</t>
+          <t>Paper or pad holder or dispensers</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>MSP-FM-CATL4-645</t>
+          <t>BSP-HRES-CATL4-039</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>CLEANING SUPPLIES</t>
+          <t>GENERAL OFFICE SUPPLIES</t>
         </is>
       </c>
     </row>
@@ -3006,22 +3006,22 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>N90101603</t>
+          <t>N78100000</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Catering services</t>
+          <t>Mail and cargo transport</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>BSP-HRES-CATL4-031</t>
+          <t>LSP-WWLAPEX-CATL2-021</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>CATERING</t>
+          <t>AIR, PARCEL, EXPRESS, GLOBAL TRADE SERVICES</t>
         </is>
       </c>
     </row>
@@ -3033,22 +3033,22 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>N40161505</t>
+          <t>N78121603</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Air filters</t>
+          <t>Freight fee</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>MSP-FM-CATL4-630</t>
+          <t>LSP-WWLOWS-CATL4-323</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>FACILITIES REPAIR - FILTRATION SYSTEMS - MATERIALS</t>
+          <t>HANDLING FEES, WHSE</t>
         </is>
       </c>
     </row>
@@ -3060,22 +3060,22 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>N47131805</t>
+          <t>N24122001</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>General purpose cleaners</t>
+          <t>Squeeze bottles</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>MSP-FM-CATL4-645</t>
+          <t>MSP-WWP-CATL4-982</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>CLEANING SUPPLIES</t>
+          <t>PACKAGING ACCESSORIES MISCELLANEOUS</t>
         </is>
       </c>
     </row>
@@ -3087,22 +3087,22 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>N31211903</t>
+          <t>N78100000</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Masking equipment</t>
+          <t>Mail and cargo transport</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>MSP-PFE-CATL4-841</t>
+          <t>LSP-WWLAPEX-CATL2-021</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>PAINT CONSUMABLES</t>
+          <t>AIR, PARCEL, EXPRESS, GLOBAL TRADE SERVICES</t>
         </is>
       </c>
     </row>
@@ -3141,22 +3141,22 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>N47131805</t>
+          <t>N49101701</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>General purpose cleaners</t>
+          <t>Medals</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>MSP-FM-CATL4-645</t>
+          <t>BSP-MCS-CATL4-278</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>CLEANING SUPPLIES</t>
+          <t>TRADEMARKED PROMOTIONAL PRODUCTS</t>
         </is>
       </c>
     </row>

</xml_diff>